<commit_message>
Add missing resistors on v0.4.1 BOM
</commit_message>
<xml_diff>
--- a/reference/hardware/v0.4/v0.4.1_bom.xlsx
+++ b/reference/hardware/v0.4/v0.4.1_bom.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27106"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27214"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -447,9 +447,6 @@
     <t>160-1139-ND</t>
   </si>
   <si>
-    <t>R10,13,16,19,23,24,29,30,50,51,57,58</t>
-  </si>
-  <si>
     <t>Battery reference (Voltage divider)</t>
   </si>
   <si>
@@ -561,9 +558,6 @@
     <t>Included</t>
   </si>
   <si>
-    <t>R10,13,23,24,50,51,57,58</t>
-  </si>
-  <si>
     <t>Q1,2,5,6,7,8</t>
   </si>
   <si>
@@ -874,6 +868,12 @@
   </si>
   <si>
     <t>D15,17</t>
+  </si>
+  <si>
+    <t>R10,13,16,19,23,24,29,30,50,51,57,58,59,60</t>
+  </si>
+  <si>
+    <t>R10,13,23,24,50,51,57,58,59,60</t>
   </si>
 </sst>
 </file>
@@ -1203,17 +1203,17 @@
     <xf numFmtId="164" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -1609,8 +1609,8 @@
   </sheetPr>
   <dimension ref="A1:Y53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1630,16 +1630,16 @@
   <sheetData>
     <row r="1" spans="1:25" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="D1" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>198</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -1651,7 +1651,7 @@
         <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>3</v>
@@ -1660,7 +1660,7 @@
         <v>4</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>5</v>
@@ -1669,40 +1669,40 @@
         <v>6</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>216</v>
-      </c>
       <c r="Q1" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="V1" s="21" t="s">
+        <v>209</v>
+      </c>
+      <c r="W1" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="X1" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="Y1" s="21" t="s">
         <v>211</v>
-      </c>
-      <c r="W1" s="21" t="s">
-        <v>212</v>
-      </c>
-      <c r="X1" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="Y1" s="21" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1759,7 +1759,7 @@
         <v>8</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>9</v>
@@ -1772,16 +1772,16 @@
         <v>13</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="O3" s="5">
         <v>1.7</v>
@@ -1842,7 +1842,7 @@
         <v>11</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>12</v>
@@ -1855,16 +1855,16 @@
         <v>13</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="O4" s="5">
         <v>0.66</v>
@@ -1925,7 +1925,7 @@
         <v>14</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>12</v>
@@ -1938,16 +1938,16 @@
         <v>13</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="O5" s="5">
         <v>0.32</v>
@@ -2008,7 +2008,7 @@
         <v>15</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>9</v>
@@ -2021,16 +2021,16 @@
         <v>13</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="O6" s="5">
         <v>1.57</v>
@@ -2091,7 +2091,7 @@
         <v>16</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>12</v>
@@ -2104,16 +2104,16 @@
         <v>10</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="O7" s="5">
         <v>0.62</v>
@@ -2174,7 +2174,7 @@
         <v>17</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>12</v>
@@ -2187,16 +2187,16 @@
         <v>13</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="O8" s="5">
         <v>0.24</v>
@@ -2248,16 +2248,16 @@
         <v>2</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>18</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>12</v>
@@ -2270,16 +2270,16 @@
         <v>13</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="O9" s="5">
         <v>0.66</v>
@@ -2331,16 +2331,16 @@
         <v>1</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>136</v>
-      </c>
       <c r="F10" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>12</v>
@@ -2351,16 +2351,16 @@
         <v>13</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="O10" s="5">
         <v>0.25</v>
@@ -2488,7 +2488,7 @@
         <v>92</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>19</v>
@@ -2504,7 +2504,7 @@
         <v>21</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="L13" s="7" t="s">
         <v>22</v>
@@ -2513,7 +2513,7 @@
         <v>23</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="O13" s="5">
         <v>0.34</v>
@@ -2565,13 +2565,13 @@
         <v>2</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>25</v>
@@ -2587,7 +2587,7 @@
         <v>26</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="L14" s="3" t="s">
         <v>24</v>
@@ -2596,7 +2596,7 @@
         <v>27</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="O14" s="5">
         <v>0.39</v>
@@ -2651,7 +2651,7 @@
         <v>91</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>28</v>
@@ -2666,14 +2666,14 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="L15" s="3"/>
       <c r="M15" s="2" t="s">
         <v>119</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="O15" s="5">
         <v>0.47</v>
@@ -2728,7 +2728,7 @@
         <v>94</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>29</v>
@@ -2747,7 +2747,7 @@
         <v>26</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="L16" s="3" t="s">
         <v>31</v>
@@ -2756,7 +2756,7 @@
         <v>32</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="O16" s="5">
         <v>0.11</v>
@@ -2946,7 +2946,7 @@
         <v>36</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="L20" s="3" t="s">
         <v>37</v>
@@ -2955,7 +2955,7 @@
         <v>38</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="O20" s="5">
         <v>0.72</v>
@@ -3051,34 +3051,34 @@
         <v>1</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="O22" s="3">
         <v>0.40200000000000002</v>
@@ -3103,7 +3103,7 @@
         <v>0.51</v>
       </c>
       <c r="U22" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="V22" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3130,10 +3130,10 @@
         <v>5</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>39</v>
@@ -3146,16 +3146,16 @@
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="M23" s="2" t="s">
         <v>109</v>
       </c>
       <c r="N23" s="3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="O23" s="5">
         <v>0.1</v>
@@ -3211,10 +3211,10 @@
         <v>114</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -3222,19 +3222,19 @@
         <v>1</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N24" s="28" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="O24" s="6">
         <v>0.56000000000000005</v>
@@ -3259,7 +3259,7 @@
         <v>5.9</v>
       </c>
       <c r="U24" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="V24" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3278,7 +3278,7 @@
         <v>782-A000026|2</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" ht="53" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20">
         <v>1</v>
       </c>
@@ -3286,16 +3286,16 @@
         <v>1</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -3303,19 +3303,19 @@
         <v>1</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="M25" s="15" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="O25" s="6">
         <v>1.1299999999999999</v>
@@ -3448,10 +3448,10 @@
         <v>116</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>107</v>
@@ -3467,7 +3467,7 @@
         <v>40</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="L28" s="3" t="s">
         <v>108</v>
@@ -3476,7 +3476,7 @@
         <v>106</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="O28" s="6">
         <v>1.51</v>
@@ -3598,10 +3598,10 @@
         <v>3</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>41</v>
@@ -3618,7 +3618,7 @@
         <v>43</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="L31" s="3" t="s">
         <v>44</v>
@@ -3627,7 +3627,7 @@
         <v>45</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="O31" s="5">
         <v>0.08</v>
@@ -3672,17 +3672,17 @@
     <row r="32" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="20">
         <f>LEN(C32)-LEN(SUBSTITUTE(C32,",",""))+1</f>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B32" s="20">
         <f t="shared" si="20"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>120</v>
+        <v>261</v>
       </c>
       <c r="D32" s="25" t="s">
-        <v>158</v>
+        <v>262</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>46</v>
@@ -3699,7 +3699,7 @@
         <v>43</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="L32" s="3" t="s">
         <v>48</v>
@@ -3708,7 +3708,7 @@
         <v>49</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="O32" s="5">
         <v>0.06</v>
@@ -3718,36 +3718,36 @@
       </c>
       <c r="Q32" s="6">
         <f t="shared" si="21"/>
-        <v>0.72</v>
+        <v>0.84</v>
       </c>
       <c r="R32" s="6">
         <f t="shared" si="4"/>
-        <v>1.32</v>
+        <v>1.54</v>
       </c>
       <c r="S32" s="6">
         <f t="shared" si="22"/>
-        <v>0.48</v>
+        <v>0.6</v>
       </c>
       <c r="T32" s="6">
         <f t="shared" si="5"/>
-        <v>0.88</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="U32" s="4"/>
       <c r="V32" s="4" t="str">
         <f t="shared" si="18"/>
-        <v>12,1.00KXBK-ND</v>
+        <v>14,1.00KXBK-ND</v>
       </c>
       <c r="W32" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>8,1.00KXBK-ND</v>
+        <v>10,1.00KXBK-ND</v>
       </c>
       <c r="X32" t="str">
         <f t="shared" ref="X32:X39" si="23">"Resistor - " &amp; A32&amp;"x "&amp;E32</f>
-        <v>Resistor - 12x 1k</v>
+        <v>Resistor - 14x 1k</v>
       </c>
       <c r="Y32" t="str">
         <f t="shared" si="8"/>
-        <v>71-RN60D-F-1.0K|12</v>
+        <v>71-RN60D-F-1.0K|14</v>
       </c>
     </row>
     <row r="33" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3763,29 +3763,29 @@
         <v>115</v>
       </c>
       <c r="D33" s="26" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E33" s="13">
         <v>680</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="13"/>
       <c r="I33" s="13"/>
       <c r="J33" s="13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="K33" s="13" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="L33" s="7"/>
       <c r="M33" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="O33" s="14">
         <v>0.22</v>
@@ -3810,7 +3810,7 @@
         <v>0.6</v>
       </c>
       <c r="U33" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="V33" s="4" t="str">
         <f t="shared" si="18"/>
@@ -3839,10 +3839,10 @@
         <v>6</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E34" s="3">
         <v>470</v>
@@ -3859,7 +3859,7 @@
         <v>51</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="L34" s="7" t="s">
         <v>52</v>
@@ -3868,7 +3868,7 @@
         <v>53</v>
       </c>
       <c r="N34" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="O34" s="5">
         <v>0.11</v>
@@ -3925,7 +3925,7 @@
         <v>85</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>54</v>
@@ -3941,7 +3941,7 @@
         <v>56</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="L35" s="3" t="s">
         <v>57</v>
@@ -3950,7 +3950,7 @@
         <v>58</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="O35" s="5">
         <v>1.92</v>
@@ -4007,7 +4007,7 @@
         <v>86</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>59</v>
@@ -4021,7 +4021,7 @@
         <v>43</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="L36" s="3" t="s">
         <v>60</v>
@@ -4030,7 +4030,7 @@
         <v>61</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="O36" s="5">
         <v>0.46</v>
@@ -4055,7 +4055,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="U36" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="V36" s="4" t="str">
         <f t="shared" si="18"/>
@@ -4089,7 +4089,7 @@
         <v>87</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>62</v>
@@ -4103,7 +4103,7 @@
         <v>43</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="L37" s="3" t="s">
         <v>63</v>
@@ -4112,7 +4112,7 @@
         <v>64</v>
       </c>
       <c r="N37" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="O37" s="5">
         <v>0.46</v>
@@ -4137,7 +4137,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="U37" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="V37" s="4" t="str">
         <f t="shared" si="18"/>
@@ -4166,10 +4166,10 @@
         <v>8</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D38" s="25" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>65</v>
@@ -4186,7 +4186,7 @@
         <v>43</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="L38" s="3" t="s">
         <v>67</v>
@@ -4195,7 +4195,7 @@
         <v>68</v>
       </c>
       <c r="N38" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="O38" s="5">
         <v>0.1</v>
@@ -4250,7 +4250,7 @@
         <v>88</v>
       </c>
       <c r="D39" s="25" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E39" s="3">
         <v>160</v>
@@ -4267,7 +4267,7 @@
         <v>43</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="L39" s="3" t="s">
         <v>70</v>
@@ -4276,7 +4276,7 @@
         <v>71</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="O39" s="5">
         <v>0.27</v>
@@ -4419,7 +4419,7 @@
         <v>77</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="L42" s="3" t="s">
         <v>74</v>
@@ -4428,7 +4428,7 @@
         <v>74</v>
       </c>
       <c r="N42" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="O42" s="5">
         <v>1.68</v>
@@ -4485,7 +4485,7 @@
         <v>98</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>97</v>
@@ -4502,13 +4502,13 @@
       </c>
       <c r="K43" s="3"/>
       <c r="L43" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="M43" s="2" t="s">
         <v>95</v>
       </c>
       <c r="N43" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="O43" s="6">
         <v>15.41</v>
@@ -4559,19 +4559,19 @@
         <v>1</v>
       </c>
       <c r="C44" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="E44" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="D44" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="E44" s="13" t="s">
+      <c r="F44" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="F44" s="13" t="s">
+      <c r="G44" s="3" t="s">
         <v>154</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>155</v>
       </c>
       <c r="H44" s="13"/>
       <c r="I44" s="13">
@@ -4581,16 +4581,16 @@
         <v>78</v>
       </c>
       <c r="K44" s="13" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="L44" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M44" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N44" s="13" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="O44" s="23">
         <v>2.92</v>
@@ -4636,42 +4636,42 @@
       <c r="A45" s="20">
         <v>1</v>
       </c>
-      <c r="B45" s="33">
+      <c r="B45" s="31">
         <v>1</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H45" s="13"/>
       <c r="I45" s="13">
         <v>1</v>
       </c>
       <c r="J45" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="K45" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="L45" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="M45" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="N45" s="2" t="s">
         <v>259</v>
-      </c>
-      <c r="K45" s="32" t="s">
-        <v>193</v>
-      </c>
-      <c r="L45" s="13" t="s">
-        <v>257</v>
-      </c>
-      <c r="M45" s="13" t="s">
-        <v>260</v>
-      </c>
-      <c r="N45" s="2" t="s">
-        <v>261</v>
       </c>
       <c r="O45" s="6">
         <v>2.4</v>
@@ -4727,7 +4727,7 @@
         <v>101</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
@@ -4735,7 +4735,7 @@
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
       <c r="K46" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="L46" s="3" t="s">
         <v>100</v>
@@ -4744,7 +4744,7 @@
         <v>99</v>
       </c>
       <c r="N46" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="O46" s="6">
         <v>0.5</v>
@@ -4829,10 +4829,10 @@
         <v>1</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
@@ -4842,17 +4842,17 @@
         <v>1</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="K48" s="3"/>
       <c r="L48" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="M48" s="13" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="N48" s="13" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O48" s="6">
         <v>15.33</v>
@@ -4962,10 +4962,10 @@
       </c>
       <c r="B51" s="17"/>
       <c r="C51" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>82</v>
@@ -5055,10 +5055,10 @@
       <c r="I53" s="8"/>
       <c r="J53" s="4"/>
       <c r="K53" s="8"/>
-      <c r="L53" s="30" t="s">
+      <c r="L53" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="M53" s="31"/>
+      <c r="M53" s="33"/>
       <c r="N53" s="27"/>
       <c r="O53" s="1" t="s">
         <v>79</v>
@@ -5066,19 +5066,19 @@
       <c r="P53" s="1"/>
       <c r="Q53" s="11">
         <f>SUM(Q2:Q52)</f>
-        <v>100.75200000000001</v>
+        <v>100.87200000000001</v>
       </c>
       <c r="R53" s="11">
         <f>SUM(R2:R52)</f>
-        <v>102.88000000000001</v>
+        <v>103.10000000000001</v>
       </c>
       <c r="S53" s="11">
         <f>SUM(S2:S52)</f>
-        <v>74.492000000000004</v>
+        <v>74.612000000000009</v>
       </c>
       <c r="T53" s="11">
         <f>SUM(T2:T52)</f>
-        <v>78.660000000000011</v>
+        <v>78.88000000000001</v>
       </c>
       <c r="U53" s="10" t="s">
         <v>80</v>

</xml_diff>